<commit_message>
Updates to stations, images and location sheets
</commit_message>
<xml_diff>
--- a/LOCATION SHEETS/1830sLOCATIONS.xlsx
+++ b/LOCATION SHEETS/1830sLOCATIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/WR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658AF60-C05D-9743-B3E6-35BE70AD2EE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2614C550-C63B-C141-8EB3-E724D07EDC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="28100" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="341">
   <si>
     <t>LOCATIONS IN 1830s</t>
   </si>
@@ -1820,6 +1820,15 @@
   </si>
   <si>
     <t>RR259</t>
+  </si>
+  <si>
+    <t>RR316</t>
+  </si>
+  <si>
+    <t>RR321</t>
+  </si>
+  <si>
+    <t>RR453</t>
   </si>
 </sst>
 </file>
@@ -2423,8 +2432,8 @@
   <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="6" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3030,6 +3039,9 @@
       <c r="F22" s="25" t="s">
         <v>18</v>
       </c>
+      <c r="G22" s="40" t="s">
+        <v>339</v>
+      </c>
       <c r="J22" s="25" t="s">
         <v>72</v>
       </c>
@@ -3050,6 +3062,9 @@
       <c r="E23" s="24"/>
       <c r="F23" s="25" t="s">
         <v>18</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>339</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>75</v>
@@ -4215,6 +4230,9 @@
       <c r="F73" s="25" t="s">
         <v>213</v>
       </c>
+      <c r="G73" s="40" t="s">
+        <v>340</v>
+      </c>
       <c r="H73" s="25" t="s">
         <v>223</v>
       </c>
@@ -4533,6 +4551,9 @@
       <c r="E87" s="24"/>
       <c r="F87" s="25" t="s">
         <v>18</v>
+      </c>
+      <c r="G87" t="s">
+        <v>338</v>
       </c>
       <c r="J87" s="25" t="s">
         <v>257</v>

</xml_diff>